<commit_message>
PerFormance inport data and show
</commit_message>
<xml_diff>
--- a/data/설비 가동율.xlsx
+++ b/data/설비 가동율.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="11550" tabRatio="624"/>
+    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="11550" tabRatio="624" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="젯팅 장비" sheetId="44" r:id="rId1"/>
@@ -817,7 +817,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -942,6 +942,27 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -959,24 +980,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1296,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Y22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -1359,56 +1362,56 @@
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="2:25" ht="24" customHeight="1">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="48" t="s">
+      <c r="H4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="48" t="s">
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="49"/>
-      <c r="S4" s="50"/>
-      <c r="T4" s="48" t="s">
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="U4" s="49"/>
-      <c r="V4" s="49"/>
-      <c r="W4" s="49"/>
-      <c r="X4" s="49"/>
-      <c r="Y4" s="50"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="44"/>
+      <c r="Y4" s="45"/>
     </row>
     <row r="5" spans="2:25" ht="36" customHeight="1">
-      <c r="B5" s="43"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="53"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="8" t="s">
         <v>3</v>
       </c>
@@ -1573,7 +1576,7 @@
         <v>14567</v>
       </c>
       <c r="L7" s="37">
-        <f t="shared" ref="L6:L11" si="3">(K7/J7)*0.85</f>
+        <f t="shared" ref="L7:L11" si="3">(K7/J7)*0.85</f>
         <v>0.59060928731762063</v>
       </c>
       <c r="M7" s="37" t="s">
@@ -1937,7 +1940,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="2:11">
+    <row r="17" spans="2:21">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1945,15 +1948,15 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="2:11">
+    <row r="18" spans="2:21">
       <c r="B18" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="54" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
       <c r="F18" s="40">
         <v>45665</v>
       </c>
@@ -1970,7 +1973,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:21">
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
         <v>141</v>
@@ -1988,7 +1991,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:21">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1996,15 +1999,16 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:21">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="2:11">
+      <c r="U21" s="42"/>
+    </row>
+    <row r="22" spans="2:21">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -2014,16 +2018,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C18:E18"/>
     <mergeCell ref="T4:Y4"/>
     <mergeCell ref="H4:M4"/>
     <mergeCell ref="N4:S4"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C18:E18"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2099,41 +2103,41 @@
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="2:14" ht="24" customHeight="1">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="48" t="s">
+      <c r="H4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="50"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="45"/>
     </row>
     <row r="5" spans="2:14" ht="36" customHeight="1">
-      <c r="B5" s="43"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="58"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="59"/>
       <c r="H5" s="8" t="s">
         <v>3</v>
       </c>
@@ -2382,76 +2386,76 @@
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="2:14">
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
     </row>
     <row r="15" spans="2:14">
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
     </row>
     <row r="16" spans="2:14">
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2474,7 +2478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2535,40 +2539,40 @@
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="2:13" ht="24" customHeight="1">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="55" t="s">
         <v>133</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="48" t="s">
+      <c r="H4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="50"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="45"/>
     </row>
     <row r="5" spans="2:13" ht="36" customHeight="1">
-      <c r="B5" s="43"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="60"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="61"/>
       <c r="H5" s="8" t="s">
         <v>3</v>
       </c>
@@ -2978,44 +2982,44 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:14" ht="24" customHeight="1">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="54" t="s">
+      <c r="H4" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="48" t="s">
+      <c r="I4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="50"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="45"/>
     </row>
     <row r="5" spans="2:14" ht="36" customHeight="1">
-      <c r="B5" s="43"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="58"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="59"/>
       <c r="I5" s="8" t="s">
         <v>3</v>
       </c>
@@ -3352,32 +3356,32 @@
       </c>
     </row>
     <row r="5" spans="2:11" ht="24" customHeight="1">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="50"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="45"/>
     </row>
     <row r="6" spans="2:11" ht="36" customHeight="1">
-      <c r="B6" s="43"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="53"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="48"/>
       <c r="F6" s="8" t="s">
         <v>3</v>
       </c>
@@ -3727,32 +3731,32 @@
       </c>
     </row>
     <row r="5" spans="2:11" ht="24" customHeight="1">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="50"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="45"/>
     </row>
     <row r="6" spans="2:11" ht="36" customHeight="1">
-      <c r="B6" s="43"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="53"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="48"/>
       <c r="F6" s="8" t="s">
         <v>3</v>
       </c>

</xml_diff>